<commit_message>
Added full season data and another type of plot
</commit_message>
<xml_diff>
--- a/Stats/2022_GandyGoose_Stats.xlsx
+++ b/Stats/2022_GandyGoose_Stats.xlsx
@@ -80,7 +80,7 @@
     <t>Jeremy Vargas</t>
   </si>
   <si>
-    <t xml:space="preserve">Trevor Kilgannon </t>
+    <t>Trevor Kilgannon</t>
   </si>
   <si>
     <t>Fiona Harrison</t>
@@ -95,7 +95,7 @@
     <t>Charlie Ramos</t>
   </si>
   <si>
-    <t xml:space="preserve">Josh Zylstra </t>
+    <t>Josh Zylstra</t>
   </si>
   <si>
     <t>Kevin Fiedler</t>

</xml_diff>